<commit_message>
testing scrape real links
</commit_message>
<xml_diff>
--- a/FacebookPages.xlsx
+++ b/FacebookPages.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>LINK</t>
   </si>
@@ -31,55 +31,295 @@
     <t>PAGE STATUS</t>
   </si>
   <si>
-    <t>https://www.facebook.com/risacookware</t>
-  </si>
-  <si>
-    <t>Risa Verified account</t>
-  </si>
-  <si>
-    <t>678</t>
-  </si>
-  <si>
-    <t>Kitchen/cooking</t>
-  </si>
-  <si>
-    <t>October 22, 2023</t>
+    <t>https://www.facebook.com/PresidentLeniRobredoSupporters</t>
+  </si>
+  <si>
+    <t>President Leni Robredo Supporters</t>
+  </si>
+  <si>
+    <t>19K</t>
+  </si>
+  <si>
+    <t>Political Organization</t>
+  </si>
+  <si>
+    <t>November 9, 2022</t>
   </si>
   <si>
     <t>Not Active</t>
   </si>
   <si>
-    <t>https://www.facebook.com/SOICTDigitalMediaPublication</t>
-  </si>
-  <si>
-    <t>ICTzen</t>
-  </si>
-  <si>
-    <t>3.5K</t>
-  </si>
-  <si>
-    <t>Education website</t>
+    <t>https://www.facebook.com/Kakampinks.sanjosecsfp</t>
+  </si>
+  <si>
+    <t>KAKAMPINK's TAYO - San Jose</t>
+  </si>
+  <si>
+    <t>16K</t>
+  </si>
+  <si>
+    <t>Personal blog</t>
+  </si>
+  <si>
+    <t>January 20</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/CebuForChelDiokno</t>
+  </si>
+  <si>
+    <t>Ka-AKBAYAN Ni Chel sa Cebu 2025</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>Media/news company</t>
+  </si>
+  <si>
+    <t>April 7 at 7:35 PM</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/chelforpres</t>
+  </si>
+  <si>
+    <t>Chel Diokno For President Movement</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>Public figure</t>
+  </si>
+  <si>
+    <t>April 23, 2020</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100070093542402</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ApayaoParaKayLeni</t>
+  </si>
+  <si>
+    <t>Apayao Para Kay Leni Robredo</t>
+  </si>
+  <si>
+    <t>58K</t>
+  </si>
+  <si>
+    <t>Nonprofit organization</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100075626007483</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/IlonggoParaKayLeniRobredo</t>
+  </si>
+  <si>
+    <t>Ilonggo Para Kay Leni Robredo</t>
+  </si>
+  <si>
+    <t>11K</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>August 21, 2023</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/solidlenibicolalbay</t>
+  </si>
+  <si>
+    <t>SOLID LENI BICOL ALBAY</t>
+  </si>
+  <si>
+    <t>Community Center</t>
   </si>
   <si>
     <t>2d</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/rrose.chua19</t>
-  </si>
-  <si>
-    <t>Rose Ann Villanueva</t>
-  </si>
-  <si>
-    <t>4.7K</t>
-  </si>
-  <si>
-    <t>Digital creator</t>
-  </si>
-  <si>
-    <t>1h</t>
+    <t>https://www.facebook.com/YoungGlobalFilipinos</t>
+  </si>
+  <si>
+    <t>Young Global Filipinos for Leni</t>
+  </si>
+  <si>
+    <t>13K</t>
+  </si>
+  <si>
+    <t>Fan page</t>
+  </si>
+  <si>
+    <t>March 16</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/yardly811</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100072310573519</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/OnePinkFight</t>
+  </si>
+  <si>
+    <t>Kulay Rosas ang Bukas</t>
+  </si>
+  <si>
+    <t>March 26 at 10:18 PM</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/supportabicolandia</t>
+  </si>
+  <si>
+    <t>KULAY ROSAS ANG BUKAS</t>
+  </si>
+  <si>
+    <t>March 17</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/kulayrosasangbukaskayleni</t>
+  </si>
+  <si>
+    <t>Kulay Rosas Ang Bukas</t>
+  </si>
+  <si>
+    <t>6.3K</t>
+  </si>
+  <si>
+    <t>Media Critic</t>
+  </si>
+  <si>
+    <t>June 15, 2022</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/kakampinklenirobredopresident</t>
+  </si>
+  <si>
+    <t>Kulay Rosas Pa rin ang Bukas</t>
+  </si>
+  <si>
+    <t>4.5K</t>
+  </si>
+  <si>
+    <t>February 25</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100082438583919</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100083196797901</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100077103501805</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/PagibigAyKulayRosas</t>
+  </si>
+  <si>
+    <t>Kulay Rosas ang Pag-ibig</t>
+  </si>
+  <si>
+    <t>May 7, 2022</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100080445219138</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/RosasAngKulay</t>
+  </si>
+  <si>
+    <t>Angat Buhay Supporters</t>
+  </si>
+  <si>
+    <t>4.4K</t>
+  </si>
+  <si>
+    <t>April 10 at 9:05 PM</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/kulayrosasnabukas</t>
+  </si>
+  <si>
+    <t>3.3K</t>
+  </si>
+  <si>
+    <t>October 5, 2023</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MyPresidentLeniRobredo</t>
+  </si>
+  <si>
+    <t>Let Leni Lead</t>
+  </si>
+  <si>
+    <t>Political Candidate</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/PinkNaLangga</t>
+  </si>
+  <si>
+    <t>PINKnalangga: Iloilo Youth Network</t>
+  </si>
+  <si>
+    <t>Cause</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pinkmovementiloilo</t>
+  </si>
+  <si>
+    <t>Youth Pink Movement</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>February 11</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/OneJamindan</t>
+  </si>
+  <si>
+    <t>One Jamindan</t>
+  </si>
+  <si>
+    <t>Public &amp; Government Service</t>
+  </si>
+  <si>
+    <t>23h</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/TeddyBaguilatOfficial</t>
+  </si>
+  <si>
+    <t>Teddy Baguilat</t>
+  </si>
+  <si>
+    <t>85K</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/HumansOfPinas</t>
+  </si>
+  <si>
+    <t>Humans of Pinas</t>
+  </si>
+  <si>
+    <t>46K</t>
+  </si>
+  <si>
+    <t>February 3</t>
   </si>
 </sst>
 </file>
@@ -462,7 +702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
@@ -528,28 +768,568 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>